<commit_message>
Fix Errors on evaluation and reports
</commit_message>
<xml_diff>
--- a/Evaluation Forms/EvaluationForm.xlsx
+++ b/Evaluation Forms/EvaluationForm.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>EVALUATION FORM</t>
   </si>
@@ -23,15 +23,15 @@
     <t>Curriculum Year:</t>
   </si>
   <si>
+    <t>Student Number:</t>
+  </si>
+  <si>
+    <t>Department:</t>
+  </si>
+  <si>
     <t>Information Technology</t>
   </si>
   <si>
-    <t>Student Number:</t>
-  </si>
-  <si>
-    <t>Department:</t>
-  </si>
-  <si>
     <t>Subject ID</t>
   </si>
   <si>
@@ -53,61 +53,70 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>IPT 1</t>
-  </si>
-  <si>
-    <t>Integrative Programming and Technology 1 (Game Devt 1)</t>
+    <t>CC 4</t>
+  </si>
+  <si>
+    <t>Data Structures and Algorithms</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>IPT 101L</t>
-  </si>
-  <si>
-    <t>Integrative Programming and Technology 1 (Game Devt 1 Lab)</t>
-  </si>
-  <si>
-    <t>IT EL 2</t>
-  </si>
-  <si>
-    <t>Multimedia 2 - 3D Arts and Concepts</t>
-  </si>
-  <si>
-    <t>IT EL 2L</t>
-  </si>
-  <si>
-    <t>Multimedia 2 - 3D Arts and Concepts (Lab)</t>
-  </si>
-  <si>
-    <t>PF 102</t>
-  </si>
-  <si>
-    <t>Event Driven Programming</t>
-  </si>
-  <si>
-    <t>PF 102L</t>
-  </si>
-  <si>
-    <t>Event Driven Programming (Lab)</t>
-  </si>
-  <si>
-    <t>RESEARCH 1</t>
-  </si>
-  <si>
-    <t>Methods of Research in Computing</t>
-  </si>
-  <si>
-    <t>SIA 101</t>
-  </si>
-  <si>
-    <t>System Integration and Architecture 1</t>
-  </si>
-  <si>
-    <t>SIA 101L</t>
-  </si>
-  <si>
-    <t>System Integration and Architecture 1 (Lab)</t>
+    <t>DIGITAL 1</t>
+  </si>
+  <si>
+    <t>Digital Logic Design</t>
+  </si>
+  <si>
+    <t>FIL1</t>
+  </si>
+  <si>
+    <t>Pagsasaling Wika</t>
+  </si>
+  <si>
+    <t>IM 101</t>
+  </si>
+  <si>
+    <t>Fundamentals of Database Systems</t>
+  </si>
+  <si>
+    <t>NET 101</t>
+  </si>
+  <si>
+    <t>Networking 1</t>
+  </si>
+  <si>
+    <t>NET 101L</t>
+  </si>
+  <si>
+    <t>Networking 1 L</t>
+  </si>
+  <si>
+    <t>PATH FIT 3</t>
+  </si>
+  <si>
+    <t>INDIVIDUAL AND DUAL SPORTS</t>
+  </si>
+  <si>
+    <t>PF 101</t>
+  </si>
+  <si>
+    <t>Object Oriented Programming</t>
+  </si>
+  <si>
+    <t>PF 101L</t>
+  </si>
+  <si>
+    <t>RIZ</t>
+  </si>
+  <si>
+    <t>Life and Works of Rizal</t>
+  </si>
+  <si>
+    <t>SP 101</t>
+  </si>
+  <si>
+    <t>Social Issues and Professional Practices</t>
   </si>
 </sst>
 </file>
@@ -213,7 +222,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -248,23 +257,23 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
+      <c r="E2" s="2">
+        <v>2022</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" s="7" customFormat="1">
       <c r="A3" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2022</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="2"/>
@@ -294,7 +303,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -303,7 +312,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
@@ -311,7 +320,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
@@ -320,7 +329,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>15</v>
@@ -328,7 +337,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -337,7 +346,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -345,7 +354,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>20</v>
@@ -354,7 +363,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
@@ -362,7 +371,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
@@ -379,7 +388,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
@@ -396,7 +405,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -405,7 +414,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>15</v>
@@ -413,7 +422,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>28</v>
@@ -430,18 +439,52 @@
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sana last na to. Edit ng eval forms
</commit_message>
<xml_diff>
--- a/Evaluation Forms/EvaluationForm.xlsx
+++ b/Evaluation Forms/EvaluationForm.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>EVALUATION FORM</t>
   </si>
@@ -20,18 +20,18 @@
     <t>Name:</t>
   </si>
   <si>
+    <t>Department:</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Student Number:</t>
+  </si>
+  <si>
     <t>Curriculum Year:</t>
   </si>
   <si>
-    <t>Student Number:</t>
-  </si>
-  <si>
-    <t>Department:</t>
-  </si>
-  <si>
-    <t>Information Technology</t>
-  </si>
-  <si>
     <t>Subject ID</t>
   </si>
   <si>
@@ -53,70 +53,97 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>CC 4</t>
-  </si>
-  <si>
-    <t>Data Structures and Algorithms</t>
+    <t>CC 106</t>
+  </si>
+  <si>
+    <t>Applications Development and Emerging Technologies</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>DIGITAL 1</t>
-  </si>
-  <si>
-    <t>Digital Logic Design</t>
-  </si>
-  <si>
-    <t>FIL1</t>
-  </si>
-  <si>
-    <t>Pagsasaling Wika</t>
-  </si>
-  <si>
-    <t>IM 101</t>
-  </si>
-  <si>
-    <t>Fundamentals of Database Systems</t>
-  </si>
-  <si>
-    <t>NET 101</t>
-  </si>
-  <si>
-    <t>Networking 1</t>
-  </si>
-  <si>
-    <t>NET 101L</t>
-  </si>
-  <si>
-    <t>Networking 1 L</t>
-  </si>
-  <si>
-    <t>PATH FIT 3</t>
-  </si>
-  <si>
-    <t>INDIVIDUAL AND DUAL SPORTS</t>
-  </si>
-  <si>
-    <t>PF 101</t>
-  </si>
-  <si>
-    <t>Object Oriented Programming</t>
-  </si>
-  <si>
-    <t>PF 101L</t>
-  </si>
-  <si>
-    <t>RIZ</t>
-  </si>
-  <si>
-    <t>Life and Works of Rizal</t>
-  </si>
-  <si>
-    <t>SP 101</t>
-  </si>
-  <si>
-    <t>Social Issues and Professional Practices</t>
+    <t>CC 106L</t>
+  </si>
+  <si>
+    <t>Applications Development and Emerging Technologies (Lab)</t>
+  </si>
+  <si>
+    <t>FIL 2</t>
+  </si>
+  <si>
+    <t>Filipino sa Iba't Ibang Disiplina</t>
+  </si>
+  <si>
+    <t>IM 101L</t>
+  </si>
+  <si>
+    <t>Fundamentals of Database Systems (Lab)</t>
+  </si>
+  <si>
+    <t>IM 102</t>
+  </si>
+  <si>
+    <t>Advance Database Systems</t>
+  </si>
+  <si>
+    <t>IM 102L</t>
+  </si>
+  <si>
+    <t>Advance Database Systems (Lab)</t>
+  </si>
+  <si>
+    <t>IT EL 1</t>
+  </si>
+  <si>
+    <t>Multimedia 1 - 2D Arts and Concepts</t>
+  </si>
+  <si>
+    <t>IT EL 1L</t>
+  </si>
+  <si>
+    <t>Multimedia 1 - 2D Arts and Concepts (Lab)</t>
+  </si>
+  <si>
+    <t>MST 4</t>
+  </si>
+  <si>
+    <t>Living in the IT Era</t>
+  </si>
+  <si>
+    <t>NET 102</t>
+  </si>
+  <si>
+    <t>Networking 2</t>
+  </si>
+  <si>
+    <t>NET 102L</t>
+  </si>
+  <si>
+    <t>Networking 2 (Lab)</t>
+  </si>
+  <si>
+    <t>PATH FIT 4</t>
+  </si>
+  <si>
+    <t>TEAM SPORTS</t>
+  </si>
+  <si>
+    <t>QM</t>
+  </si>
+  <si>
+    <t>Quantitative Methods</t>
+  </si>
+  <si>
+    <t>WS 101</t>
+  </si>
+  <si>
+    <t>Web Systems and Technology 1</t>
+  </si>
+  <si>
+    <t>WS 101L</t>
+  </si>
+  <si>
+    <t>Web Systems and Technology 1 (Lab)</t>
   </si>
 </sst>
 </file>
@@ -177,9 +204,6 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" xfId="0" applyProtection="1" applyAlignment="1">
@@ -188,18 +212,18 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -207,7 +231,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,7 +249,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -230,89 +257,98 @@
   <cols>
     <col min="1" max="1" width="16" customWidth="1" style="1"/>
     <col min="2" max="2" width="13" customWidth="1" style="1"/>
-    <col min="3" max="3" width="50" customWidth="1" style="8"/>
+    <col min="3" max="3" width="50" customWidth="1" style="6"/>
     <col min="4" max="4" width="15" customWidth="1" style="1"/>
     <col min="5" max="5" width="15" customWidth="1" style="1"/>
-    <col min="6" max="6" width="13" customWidth="1" style="11"/>
+    <col min="6" max="6" width="13" customWidth="1" style="10"/>
     <col min="7" max="7" width="13" customWidth="1" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="2" customFormat="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" s="7" customFormat="1">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" s="9" customFormat="1">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" s="9" customFormat="1">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9">
         <v>2022</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" s="7" customFormat="1">
-      <c r="A3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="5" s="4" customFormat="1">
-      <c r="A5" s="5" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" s="6" customFormat="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" s="3" customFormat="1">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
@@ -320,16 +356,16 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>15</v>
@@ -337,12 +373,12 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="1">
@@ -354,16 +390,16 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
@@ -371,12 +407,12 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="1">
@@ -388,12 +424,12 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="1">
@@ -405,12 +441,12 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="1">
@@ -422,16 +458,16 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>15</v>
@@ -439,16 +475,16 @@
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>29</v>
+      <c r="C14" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>15</v>
@@ -456,16 +492,16 @@
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="C15" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="D15" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>15</v>
@@ -473,18 +509,86 @@
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="C16" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1">
         <v>3</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -492,8 +596,8 @@
   <mergeCells>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <headerFooter/>

</xml_diff>